<commit_message>
update ejamit test output and various unit tests
</commit_message>
<xml_diff>
--- a/inst/testdata/examples_of_output/testoutput_ejamit_10pts_1miles.xlsx
+++ b/inst/testdata/examples_of_output/testoutput_ejamit_10pts_1miles.xlsx
@@ -2630,6 +2630,9 @@
     <t xml:space="preserve">US percentile for EJ Index for Particulate Matter</t>
   </si>
   <si>
+    <t xml:space="preserve">76</t>
+  </si>
+  <si>
     <t xml:space="preserve">US percentile for EJ Index for Ozone</t>
   </si>
   <si>
@@ -2696,9 +2699,6 @@
     <t xml:space="preserve">US percentile for Supplemental EJ Index for Diesel Particulate Matter</t>
   </si>
   <si>
-    <t xml:space="preserve">76</t>
-  </si>
-  <si>
     <t xml:space="preserve">US percentile for Supplemental EJ Index for Toxic Releases to Air</t>
   </si>
   <si>
@@ -3047,7 +3047,7 @@
     <t xml:space="preserve">US type of raw score for Particulate Matter EJ Index</t>
   </si>
   <si>
-    <t xml:space="preserve">121.441</t>
+    <t xml:space="preserve">102.211</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Ozone EJ Index</t>
@@ -3113,7 +3113,7 @@
     <t xml:space="preserve">US type of raw score for Wastewater Discharge EJ Index</t>
   </si>
   <si>
-    <t xml:space="preserve">10.825</t>
+    <t xml:space="preserve">10.821</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Drinking Water Non-Compliance EJ Index</t>
@@ -3125,7 +3125,7 @@
     <t xml:space="preserve">State type of raw score for Particulate Matter EJ Index</t>
   </si>
   <si>
-    <t xml:space="preserve">110.472</t>
+    <t xml:space="preserve">71.549</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Ozone EJ Index</t>
@@ -3161,7 +3161,7 @@
     <t xml:space="preserve">State type of raw score for Lead Paint EJ Index</t>
   </si>
   <si>
-    <t xml:space="preserve">143.983</t>
+    <t xml:space="preserve">143.981</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Superfund Proximity EJ Index</t>
@@ -3191,7 +3191,7 @@
     <t xml:space="preserve">State type of raw score for Wastewater Discharge EJ Index</t>
   </si>
   <si>
-    <t xml:space="preserve">12.691</t>
+    <t xml:space="preserve">12.69</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Drinking Water Non-Compliance EJ Index</t>
@@ -3203,7 +3203,7 @@
     <t xml:space="preserve">US type of raw score for Particulate Matter Supplemental EJ Index</t>
   </si>
   <si>
-    <t xml:space="preserve">122.523</t>
+    <t xml:space="preserve">103.974</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Ozone Supplemental EJ Index</t>
@@ -3269,7 +3269,7 @@
     <t xml:space="preserve">US type of raw score for Wastewater Discharge Supplemental EJ Index</t>
   </si>
   <si>
-    <t xml:space="preserve">14.414</t>
+    <t xml:space="preserve">14.408</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Drinking Water Non-Compliance Supplemental EJ Index</t>
@@ -3281,7 +3281,7 @@
     <t xml:space="preserve">State type of raw score for Particulate Matter Supplemental EJ Index</t>
   </si>
   <si>
-    <t xml:space="preserve">100.312</t>
+    <t xml:space="preserve">63.229</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Ozone Supplemental EJ Index</t>
@@ -3317,7 +3317,7 @@
     <t xml:space="preserve">State type of raw score for Lead Paint Supplemental EJ Index</t>
   </si>
   <si>
-    <t xml:space="preserve">128.183</t>
+    <t xml:space="preserve">128.182</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Superfund Proximity Supplemental EJ Index</t>
@@ -3347,7 +3347,7 @@
     <t xml:space="preserve">State type of raw score for Wastewater Discharge Supplemental EJ Index</t>
   </si>
   <si>
-    <t xml:space="preserve">14.286</t>
+    <t xml:space="preserve">14.285</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Drinking Water Non-Compliance Supplemental EJ Index</t>
@@ -5015,52 +5015,52 @@
         <v>868</v>
       </c>
       <c r="JJ1" s="17" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="JK1" s="17" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="JL1" s="17" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="JM1" s="17" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="JN1" s="17" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="JO1" s="17" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="JP1" s="17" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="JQ1" s="17" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="JR1" s="17" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="JS1" s="17" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="JT1" s="17" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="JU1" s="17" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="JV1" s="17" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="JW1" s="17" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="JX1" s="17" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="JY1" s="17" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="JZ1" s="17" t="s">
         <v>892</v>
@@ -6243,7 +6243,7 @@
         <v>65</v>
       </c>
       <c r="JJ2" s="27" t="n">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="JK2" s="27" t="n">
         <v>45</v>
@@ -6282,7 +6282,7 @@
         <v>61</v>
       </c>
       <c r="JW2" s="27" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="JX2" s="27" t="n">
         <v>35</v>
@@ -6531,7 +6531,7 @@
         <v>76.952104370838</v>
       </c>
       <c r="NB2" s="23" t="n">
-        <v>22.4936920468603</v>
+        <v>7.10327117269274</v>
       </c>
       <c r="NC2" s="23" t="n">
         <v>40.0868661456388</v>
@@ -6555,7 +6555,7 @@
         <v>0</v>
       </c>
       <c r="NJ2" s="23" t="n">
-        <v>0.112202606408331</v>
+        <v>0.11220260640833</v>
       </c>
       <c r="NK2" s="23" t="n">
         <v>69.4594241523752</v>
@@ -6570,7 +6570,7 @@
         <v>32.5272085203054</v>
       </c>
       <c r="NO2" s="23" t="n">
-        <v>48.7908127804582</v>
+        <v>4.64674407432935</v>
       </c>
       <c r="NP2" s="23" t="n">
         <v>67.1034011881344</v>
@@ -6609,7 +6609,7 @@
         <v>88.2876496374691</v>
       </c>
       <c r="OB2" s="23" t="n">
-        <v>25.8071591247987</v>
+        <v>8.14962919730484</v>
       </c>
       <c r="OC2" s="23" t="n">
         <v>45.5515987340029</v>
@@ -6648,7 +6648,7 @@
         <v>29.6120790719457</v>
       </c>
       <c r="OO2" s="23" t="n">
-        <v>44.4181186079186</v>
+        <v>4.23029701027796</v>
       </c>
       <c r="OP2" s="23" t="n">
         <v>60.5340087444893</v>
@@ -7479,7 +7479,7 @@
         <v>78</v>
       </c>
       <c r="JJ3" s="27" t="n">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="JK3" s="27" t="n">
         <v>54</v>
@@ -7518,7 +7518,7 @@
         <v>83</v>
       </c>
       <c r="JW3" s="27" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="JX3" s="27" t="n">
         <v>48</v>
@@ -7767,7 +7767,7 @@
         <v>117.323328112055</v>
       </c>
       <c r="NB3" s="23" t="n">
-        <v>3.14198123056293</v>
+        <v>17.011654439911</v>
       </c>
       <c r="NC3" s="23" t="n">
         <v>55.4040107256464</v>
@@ -7806,7 +7806,7 @@
         <v>100.1875317907</v>
       </c>
       <c r="NO3" s="23" t="n">
-        <v>9.08260253494678</v>
+        <v>21.6245670015017</v>
       </c>
       <c r="NP3" s="23" t="n">
         <v>107.773014854969</v>
@@ -7845,7 +7845,7 @@
         <v>137.704563137612</v>
       </c>
       <c r="OB3" s="23" t="n">
-        <v>3.69086287583923</v>
+        <v>19.9724899609038</v>
       </c>
       <c r="OC3" s="23" t="n">
         <v>63.8425278565321</v>
@@ -7884,7 +7884,7 @@
         <v>116.075166654765</v>
       </c>
       <c r="OO3" s="23" t="n">
-        <v>10.5269105847758</v>
+        <v>24.9473534986623</v>
       </c>
       <c r="OP3" s="23" t="n">
         <v>123.809912115067</v>
@@ -8715,7 +8715,7 @@
         <v>49</v>
       </c>
       <c r="JJ4" s="27" t="n">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="JK4" s="27" t="n">
         <v>45</v>
@@ -8754,7 +8754,7 @@
         <v>55</v>
       </c>
       <c r="JW4" s="27" t="n">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="JX4" s="27" t="n">
         <v>51</v>
@@ -9003,7 +9003,7 @@
         <v>46.2569024602887</v>
       </c>
       <c r="NB4" s="23" t="n">
-        <v>57.7881992700524</v>
+        <v>53.1939097284581</v>
       </c>
       <c r="NC4" s="23" t="n">
         <v>40.6174315726002</v>
@@ -9015,7 +9015,7 @@
         <v>50.5458394252474</v>
       </c>
       <c r="NF4" s="23" t="n">
-        <v>25.6727508551649</v>
+        <v>25.6727508551648</v>
       </c>
       <c r="NG4" s="23" t="n">
         <v>32.4640947364053</v>
@@ -9042,7 +9042,7 @@
         <v>28.9204926360807</v>
       </c>
       <c r="NO4" s="23" t="n">
-        <v>30.1242536215768</v>
+        <v>32.4176693416491</v>
       </c>
       <c r="NP4" s="23" t="n">
         <v>25.5731126250819</v>
@@ -9081,13 +9081,13 @@
         <v>78.7006513591159</v>
       </c>
       <c r="OB4" s="23" t="n">
-        <v>98.2919233098529</v>
+        <v>90.4794216105559</v>
       </c>
       <c r="OC4" s="23" t="n">
         <v>68.6958772623984</v>
       </c>
       <c r="OD4" s="23" t="n">
-        <v>62.5362827891599</v>
+        <v>62.53628278916</v>
       </c>
       <c r="OE4" s="23" t="n">
         <v>85.95796252536</v>
@@ -9099,7 +9099,7 @@
         <v>54.3079386002305</v>
       </c>
       <c r="OH4" s="23" t="n">
-        <v>0.340712220215132</v>
+        <v>0.340712220215133</v>
       </c>
       <c r="OI4" s="23" t="n">
         <v>44.7075980646423</v>
@@ -9120,7 +9120,7 @@
         <v>40.0105653644774</v>
       </c>
       <c r="OO4" s="23" t="n">
-        <v>41.5311198776367</v>
+        <v>44.7470796119325</v>
       </c>
       <c r="OP4" s="23" t="n">
         <v>35.036702621778</v>
@@ -9951,7 +9951,7 @@
         <v>68</v>
       </c>
       <c r="JJ5" s="27" t="n">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="JK5" s="27" t="n">
         <v>64</v>
@@ -9990,7 +9990,7 @@
         <v>56</v>
       </c>
       <c r="JW5" s="27" t="n">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="JX5" s="27" t="n">
         <v>53</v>
@@ -10239,7 +10239,7 @@
         <v>85.7940962185773</v>
       </c>
       <c r="NB5" s="23" t="n">
-        <v>78.1608849503045</v>
+        <v>37.3024409358371</v>
       </c>
       <c r="NC5" s="23" t="n">
         <v>77.9065108076848</v>
@@ -10278,7 +10278,7 @@
         <v>58.3104575189475</v>
       </c>
       <c r="NO5" s="23" t="n">
-        <v>39.3662659394878</v>
+        <v>24.285683048698</v>
       </c>
       <c r="NP5" s="23" t="n">
         <v>83.7855642707251</v>
@@ -10314,10 +10314,10 @@
         <v>0</v>
       </c>
       <c r="OA5" s="23" t="n">
-        <v>79.2572403521154</v>
+        <v>79.2572403521155</v>
       </c>
       <c r="OB5" s="23" t="n">
-        <v>72.1947359100883</v>
+        <v>34.4713706018905</v>
       </c>
       <c r="OC5" s="23" t="n">
         <v>71.9788398868712</v>
@@ -10356,7 +10356,7 @@
         <v>41.0599362977923</v>
       </c>
       <c r="OO5" s="23" t="n">
-        <v>27.7031552536311</v>
+        <v>17.0860637170125</v>
       </c>
       <c r="OP5" s="23" t="n">
         <v>59.061514477926</v>
@@ -11187,7 +11187,7 @@
         <v>99</v>
       </c>
       <c r="JJ6" s="27" t="n">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="JK6" s="27" t="n">
         <v>98</v>
@@ -11475,7 +11475,7 @@
         <v>281.358733659431</v>
       </c>
       <c r="NB6" s="23" t="n">
-        <v>282.909022125377</v>
+        <v>262.406396881789</v>
       </c>
       <c r="NC6" s="23" t="n">
         <v>274.812565316584</v>
@@ -11514,7 +11514,7 @@
         <v>247.397482759081</v>
       </c>
       <c r="NO6" s="23" t="n">
-        <v>240.32600179043</v>
+        <v>197.755366389805</v>
       </c>
       <c r="NP6" s="23" t="n">
         <v>318.831826463656</v>
@@ -11553,7 +11553,7 @@
         <v>253.679355736826</v>
       </c>
       <c r="OB6" s="23" t="n">
-        <v>254.985590802148</v>
+        <v>236.501124771856</v>
       </c>
       <c r="OC6" s="23" t="n">
         <v>247.683878413021</v>
@@ -11592,7 +11592,7 @@
         <v>184.897571963874</v>
       </c>
       <c r="OO6" s="23" t="n">
-        <v>179.344973662782</v>
+        <v>147.672115001314</v>
       </c>
       <c r="OP6" s="23" t="n">
         <v>238.072938604179</v>
@@ -12423,7 +12423,7 @@
         <v>79</v>
       </c>
       <c r="JJ7" s="27" t="n">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="JK7" s="27" t="n">
         <v>94</v>
@@ -12462,7 +12462,7 @@
         <v>79</v>
       </c>
       <c r="JW7" s="27" t="n">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="JX7" s="27" t="n">
         <v>96</v>
@@ -12711,7 +12711,7 @@
         <v>119.342934038794</v>
       </c>
       <c r="NB7" s="23" t="n">
-        <v>140.47556642207</v>
+        <v>120.693151951277</v>
       </c>
       <c r="NC7" s="23" t="n">
         <v>226.881109944851</v>
@@ -12750,7 +12750,7 @@
         <v>214.490657324609</v>
       </c>
       <c r="NO7" s="23" t="n">
-        <v>166.375481097491</v>
+        <v>82.2969344855926</v>
       </c>
       <c r="NP7" s="23" t="n">
         <v>225.534652280655</v>
@@ -12789,7 +12789,7 @@
         <v>127.628782669497</v>
       </c>
       <c r="OB7" s="23" t="n">
-        <v>150.258028876184</v>
+        <v>128.905833428549</v>
       </c>
       <c r="OC7" s="23" t="n">
         <v>242.29122138924</v>
@@ -12828,7 +12828,7 @@
         <v>217.968064111516</v>
       </c>
       <c r="OO7" s="23" t="n">
-        <v>169.56437602125</v>
+        <v>83.5408998486035</v>
       </c>
       <c r="OP7" s="23" t="n">
         <v>228.543558431621</v>
@@ -13659,7 +13659,7 @@
         <v>92</v>
       </c>
       <c r="JJ8" s="27" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="JK8" s="27" t="n">
         <v>74</v>
@@ -13698,7 +13698,7 @@
         <v>90</v>
       </c>
       <c r="JW8" s="27" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="JX8" s="27" t="n">
         <v>67</v>
@@ -13947,7 +13947,7 @@
         <v>191.205018898703</v>
       </c>
       <c r="NB8" s="23" t="n">
-        <v>165.841087820304</v>
+        <v>171.69430268455</v>
       </c>
       <c r="NC8" s="23" t="n">
         <v>109.078326055277</v>
@@ -13986,7 +13986,7 @@
         <v>188.475055226975</v>
       </c>
       <c r="NO8" s="23" t="n">
-        <v>81.9311902905521</v>
+        <v>119.830003902458</v>
       </c>
       <c r="NP8" s="23" t="n">
         <v>81.229156086671</v>
@@ -14025,7 +14025,7 @@
         <v>167.951669108002</v>
       </c>
       <c r="OB8" s="23" t="n">
-        <v>145.672366063063</v>
+        <v>150.813743688819</v>
       </c>
       <c r="OC8" s="23" t="n">
         <v>99.0898348698581</v>
@@ -14064,7 +14064,7 @@
         <v>134.005453297153</v>
       </c>
       <c r="OO8" s="23" t="n">
-        <v>58.2491742039815</v>
+        <v>85.2020911262495</v>
       </c>
       <c r="OP8" s="23" t="n">
         <v>61.4445824420369</v>
@@ -14895,7 +14895,7 @@
         <v>27</v>
       </c>
       <c r="JJ9" s="27" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="JK9" s="27" t="n">
         <v>45</v>
@@ -14934,7 +14934,7 @@
         <v>30</v>
       </c>
       <c r="JW9" s="27" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="JX9" s="27" t="n">
         <v>57</v>
@@ -15183,7 +15183,7 @@
         <v>20.8338240073862</v>
       </c>
       <c r="NB9" s="23" t="n">
-        <v>13.6192087208813</v>
+        <v>16.2577007736515</v>
       </c>
       <c r="NC9" s="23" t="n">
         <v>41.5031106420557</v>
@@ -15216,13 +15216,13 @@
         <v>45.8075326573284</v>
       </c>
       <c r="NM9" s="23" t="n">
-        <v>54.4287172669241</v>
+        <v>54.3401515905647</v>
       </c>
       <c r="NN9" s="23" t="n">
         <v>76.8200246924354</v>
       </c>
       <c r="NO9" s="23" t="n">
-        <v>26.3966354599835</v>
+        <v>35.0423787864745</v>
       </c>
       <c r="NP9" s="23" t="n">
         <v>45.7650865975849</v>
@@ -15255,13 +15255,13 @@
         <v>83.4038301585497</v>
       </c>
       <c r="NZ9" s="23" t="n">
-        <v>76.0498181113261</v>
+        <v>76.027772567431</v>
       </c>
       <c r="OA9" s="23" t="n">
         <v>40.4442430955068</v>
       </c>
       <c r="OB9" s="23" t="n">
-        <v>26.2845715001041</v>
+        <v>31.4279734183963</v>
       </c>
       <c r="OC9" s="23" t="n">
         <v>78.3111587834872</v>
@@ -15294,13 +15294,13 @@
         <v>87.848543965725</v>
       </c>
       <c r="OM9" s="23" t="n">
-        <v>103.948171527145</v>
+        <v>103.836739761746</v>
       </c>
       <c r="ON9" s="23" t="n">
         <v>116.478675223817</v>
       </c>
       <c r="OO9" s="23" t="n">
-        <v>39.326312655874</v>
+        <v>52.0940114253976</v>
       </c>
       <c r="OP9" s="23" t="n">
         <v>67.140584360414</v>
@@ -15333,7 +15333,7 @@
         <v>125.494524497692</v>
       </c>
       <c r="OZ9" s="23" t="n">
-        <v>111.986479534127</v>
+        <v>111.953235707364</v>
       </c>
     </row>
     <row r="10">
@@ -16131,7 +16131,7 @@
         <v>40</v>
       </c>
       <c r="JJ10" s="27" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="JK10" s="27" t="n">
         <v>58</v>
@@ -16170,7 +16170,7 @@
         <v>32</v>
       </c>
       <c r="JW10" s="27" t="n">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="JX10" s="27" t="n">
         <v>57</v>
@@ -16419,7 +16419,7 @@
         <v>34.8367384887128</v>
       </c>
       <c r="NB10" s="23" t="n">
-        <v>91.7717841289426</v>
+        <v>95.4344294722853</v>
       </c>
       <c r="NC10" s="23" t="n">
         <v>63.5086082415396</v>
@@ -16431,7 +16431,7 @@
         <v>64.6306849495215</v>
       </c>
       <c r="NF10" s="23" t="n">
-        <v>56.9191126054964</v>
+        <v>56.9191126054963</v>
       </c>
       <c r="NG10" s="23" t="n">
         <v>65.9516507044135</v>
@@ -16452,13 +16452,13 @@
         <v>92.4504852183565</v>
       </c>
       <c r="NM10" s="23" t="n">
-        <v>32.1273648370011</v>
+        <v>32.127364837001</v>
       </c>
       <c r="NN10" s="23" t="n">
         <v>61.5902989919776</v>
       </c>
       <c r="NO10" s="23" t="n">
-        <v>100.32684917476</v>
+        <v>46.2678173554966</v>
       </c>
       <c r="NP10" s="23" t="n">
         <v>83.5823939937704</v>
@@ -16497,7 +16497,7 @@
         <v>43.3702089976161</v>
       </c>
       <c r="OB10" s="23" t="n">
-        <v>114.544771853045</v>
+        <v>119.179945169641</v>
       </c>
       <c r="OC10" s="23" t="n">
         <v>78.6296145938071</v>
@@ -16536,7 +16536,7 @@
         <v>52.5782117517509</v>
       </c>
       <c r="OO10" s="23" t="n">
-        <v>85.404451684061</v>
+        <v>39.3051110813093</v>
       </c>
       <c r="OP10" s="23" t="n">
         <v>71.0640541730264</v>
@@ -17367,7 +17367,7 @@
         <v>17</v>
       </c>
       <c r="JJ11" s="27" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="JK11" s="27" t="n">
         <v>23</v>
@@ -17406,7 +17406,7 @@
         <v>16</v>
       </c>
       <c r="JW11" s="27" t="n">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="JX11" s="27" t="n">
         <v>23</v>
@@ -17655,13 +17655,13 @@
         <v>11.4719784442551</v>
       </c>
       <c r="NB11" s="23" t="n">
-        <v>18.4020240303908</v>
+        <v>23.2810038753656</v>
       </c>
       <c r="NC11" s="23" t="n">
         <v>15.8294281365048</v>
       </c>
       <c r="ND11" s="23" t="n">
-        <v>27.2152039828164</v>
+        <v>27.2152039828163</v>
       </c>
       <c r="NE11" s="23" t="n">
         <v>22.7679456305678</v>
@@ -17670,7 +17670,7 @@
         <v>16.1729271888802</v>
       </c>
       <c r="NG11" s="23" t="n">
-        <v>30.8399700593178</v>
+        <v>30.8399700593177</v>
       </c>
       <c r="NH11" s="23" t="n">
         <v>12.8527927032356</v>
@@ -17682,10 +17682,10 @@
         <v>13.5146949461143</v>
       </c>
       <c r="NK11" s="23" t="n">
-        <v>33.3544873713658</v>
+        <v>33.3544873713657</v>
       </c>
       <c r="NL11" s="23" t="n">
-        <v>33.5890640983318</v>
+        <v>33.5890640983317</v>
       </c>
       <c r="NM11" s="23" t="n">
         <v>0</v>
@@ -17694,7 +17694,7 @@
         <v>11.2713427288303</v>
       </c>
       <c r="NO11" s="23" t="n">
-        <v>4.98471721830082</v>
+        <v>14.6021639810745</v>
       </c>
       <c r="NP11" s="23" t="n">
         <v>14.811463835389</v>
@@ -17712,7 +17712,7 @@
         <v>23.8865001827917</v>
       </c>
       <c r="NU11" s="23" t="n">
-        <v>2.17222936511013</v>
+        <v>2.12321394730008</v>
       </c>
       <c r="NV11" s="23" t="n">
         <v>0</v>
@@ -17733,7 +17733,7 @@
         <v>21.501400215027</v>
       </c>
       <c r="OB11" s="23" t="n">
-        <v>34.4809184087645</v>
+        <v>43.6582934703797</v>
       </c>
       <c r="OC11" s="23" t="n">
         <v>29.6242163063856</v>
@@ -17772,7 +17772,7 @@
         <v>16.8355873424264</v>
       </c>
       <c r="OO11" s="23" t="n">
-        <v>7.43027680185661</v>
+        <v>21.6983442716179</v>
       </c>
       <c r="OP11" s="23" t="n">
         <v>21.9720961019736</v>
@@ -17790,7 +17790,7 @@
         <v>35.6567565348414</v>
       </c>
       <c r="OU11" s="23" t="n">
-        <v>2.96472008395307</v>
+        <v>2.91339148915049</v>
       </c>
       <c r="OV11" s="23" t="n">
         <v>0</v>
@@ -18947,52 +18947,52 @@
         <v>868</v>
       </c>
       <c r="JH1" s="15" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="JI1" s="17" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="JJ1" s="17" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="JK1" s="17" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="JL1" s="17" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="JM1" s="17" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="JN1" s="17" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="JO1" s="17" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="JP1" s="17" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="JQ1" s="17" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="JR1" s="17" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="JS1" s="17" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="JT1" s="17" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="JU1" s="17" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="JV1" s="17" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="JW1" s="17" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="JX1" s="17" t="s">
         <v>892</v>
@@ -20173,7 +20173,7 @@
         <v>78</v>
       </c>
       <c r="JJ2" s="27" t="n">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="JK2" s="27" t="n">
         <v>83</v>
@@ -20212,7 +20212,7 @@
         <v>75</v>
       </c>
       <c r="JW2" s="27" t="n">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="JX2" s="27" t="n">
         <v>85</v>
@@ -20461,7 +20461,7 @@
         <v>117.312116899188</v>
       </c>
       <c r="NB2" s="23" t="n">
-        <v>121.440843085412</v>
+        <v>102.211035118237</v>
       </c>
       <c r="NC2" s="23" t="n">
         <v>147.749566513762</v>
@@ -20494,13 +20494,13 @@
         <v>109.501365093349</v>
       </c>
       <c r="NM2" s="23" t="n">
-        <v>10.8253658009493</v>
+        <v>10.8213053345218</v>
       </c>
       <c r="NN2" s="23" t="n">
         <v>142.891623579944</v>
       </c>
       <c r="NO2" s="23" t="n">
-        <v>110.471533216608</v>
+        <v>71.5487559652744</v>
       </c>
       <c r="NP2" s="23" t="n">
         <v>154.348158200293</v>
@@ -20518,7 +20518,7 @@
         <v>85.5078660379096</v>
       </c>
       <c r="NU2" s="23" t="n">
-        <v>143.982618644189</v>
+        <v>143.981425622932</v>
       </c>
       <c r="NV2" s="23" t="n">
         <v>162.213263447858</v>
@@ -20533,13 +20533,13 @@
         <v>108.36046751482</v>
       </c>
       <c r="NZ2" s="23" t="n">
-        <v>12.6906321431065</v>
+        <v>12.6896214220852</v>
       </c>
       <c r="OA2" s="23" t="n">
         <v>117.153378985886</v>
       </c>
       <c r="OB2" s="23" t="n">
-        <v>122.523033390055</v>
+        <v>103.973930253546</v>
       </c>
       <c r="OC2" s="23" t="n">
         <v>152.100205832046</v>
@@ -20554,7 +20554,7 @@
         <v>144.477633800058</v>
       </c>
       <c r="OG2" s="23" t="n">
-        <v>95.2776509351119</v>
+        <v>95.2776509351118</v>
       </c>
       <c r="OH2" s="23" t="n">
         <v>147.302056163125</v>
@@ -20572,13 +20572,13 @@
         <v>114.040127496428</v>
       </c>
       <c r="OM2" s="23" t="n">
-        <v>14.4135113863263</v>
+        <v>14.4084025793826</v>
       </c>
       <c r="ON2" s="23" t="n">
         <v>131.089527021018</v>
       </c>
       <c r="OO2" s="23" t="n">
-        <v>100.311668071496</v>
+        <v>63.2289343780677</v>
       </c>
       <c r="OP2" s="23" t="n">
         <v>139.762065830411</v>
@@ -20596,7 +20596,7 @@
         <v>74.1512036392973</v>
       </c>
       <c r="OU2" s="23" t="n">
-        <v>128.182861498486</v>
+        <v>128.181612175162</v>
       </c>
       <c r="OV2" s="23" t="n">
         <v>144.944179701337</v>
@@ -20611,7 +20611,7 @@
         <v>100.185422723694</v>
       </c>
       <c r="OZ2" s="23" t="n">
-        <v>14.2861597371721</v>
+        <v>14.2846356089992</v>
       </c>
     </row>
   </sheetData>
@@ -22905,10 +22905,10 @@
     </row>
     <row r="271">
       <c r="A271" t="s">
-        <v>668</v>
+        <v>869</v>
       </c>
       <c r="B271" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
     </row>
     <row r="272">
@@ -22916,7 +22916,7 @@
         <v>671</v>
       </c>
       <c r="B272" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
     </row>
     <row r="273">
@@ -22924,39 +22924,39 @@
         <v>673</v>
       </c>
       <c r="B273" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="B274" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="B275" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="B276" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="B277" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
     </row>
     <row r="278">
@@ -22964,7 +22964,7 @@
         <v>671</v>
       </c>
       <c r="B278" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
     </row>
     <row r="279">
@@ -22972,15 +22972,15 @@
         <v>673</v>
       </c>
       <c r="B279" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="B280" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
     </row>
     <row r="281">
@@ -22988,7 +22988,7 @@
         <v>642</v>
       </c>
       <c r="B281" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
     </row>
     <row r="282">
@@ -22996,23 +22996,23 @@
         <v>666</v>
       </c>
       <c r="B282" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B283" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="s">
-        <v>786</v>
+        <v>877</v>
       </c>
       <c r="B284" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="285">
@@ -23020,20 +23020,20 @@
         <v>673</v>
       </c>
       <c r="B285" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="B286" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="s">
-        <v>891</v>
+        <v>869</v>
       </c>
       <c r="B287" t="s">
         <v>892</v>
@@ -23057,7 +23057,7 @@
     </row>
     <row r="290">
       <c r="A290" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="B290" t="s">
         <v>896</v>
@@ -23065,7 +23065,7 @@
     </row>
     <row r="291">
       <c r="A291" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="B291" t="s">
         <v>897</v>
@@ -23073,7 +23073,7 @@
     </row>
     <row r="292">
       <c r="A292" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="B292" t="s">
         <v>898</v>

</xml_diff>

<commit_message>
Redid all testoutput etc since ejamit() outputs now have sitetype info
</commit_message>
<xml_diff>
--- a/inst/testdata/examples_of_output/testoutput_ejamit_10pts_1miles.xlsx
+++ b/inst/testdata/examples_of_output/testoutput_ejamit_10pts_1miles.xlsx
@@ -2630,75 +2630,75 @@
     <t xml:space="preserve">US percentile for EJ Index for Particulate Matter</t>
   </si>
   <si>
+    <t xml:space="preserve">US percentile for EJ Index for Ozone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US percentile for EJ Index for Nitrogen Dioxide (NO2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US percentile for EJ Index for Diesel Particulate Matter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US percentile for EJ Index for Toxic Releases to Air</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US percentile for EJ Index for Traffic Proximity and Volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US percentile for EJ Index for Lead Paint Indicator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US percentile for EJ Index for Superfund Proximity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US percentile for EJ Index for RMP Proximity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US percentile for EJ Index for Hazardous Waste Proximity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US percentile for EJ Index for Underground Storage Tanks (UST) indicator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US percentile for EJ Index for Wastewater Discharge Indicator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US percentile for EJ Index for Drinking Water Non-Compliance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US percentile for Supplemental EJ Index for Particulate Matter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US percentile for Supplemental EJ Index for Ozone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US percentile for Supplemental EJ Index for Nitrogen Dioxide (NO2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US percentile for Supplemental EJ Index for Diesel Particulate Matter</t>
+  </si>
+  <si>
     <t xml:space="preserve">76</t>
   </si>
   <si>
-    <t xml:space="preserve">US percentile for EJ Index for Ozone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US percentile for EJ Index for Nitrogen Dioxide (NO2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US percentile for EJ Index for Diesel Particulate Matter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US percentile for EJ Index for Toxic Releases to Air</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US percentile for EJ Index for Traffic Proximity and Volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US percentile for EJ Index for Lead Paint Indicator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">86</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US percentile for EJ Index for Superfund Proximity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US percentile for EJ Index for RMP Proximity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US percentile for EJ Index for Hazardous Waste Proximity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US percentile for EJ Index for Underground Storage Tanks (UST) indicator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US percentile for EJ Index for Wastewater Discharge Indicator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US percentile for EJ Index for Drinking Water Non-Compliance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US percentile for Supplemental EJ Index for Particulate Matter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US percentile for Supplemental EJ Index for Ozone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US percentile for Supplemental EJ Index for Nitrogen Dioxide (NO2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">87</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US percentile for Supplemental EJ Index for Diesel Particulate Matter</t>
-  </si>
-  <si>
     <t xml:space="preserve">US percentile for Supplemental EJ Index for Toxic Releases to Air</t>
   </si>
   <si>
@@ -3047,7 +3047,7 @@
     <t xml:space="preserve">US type of raw score for Particulate Matter EJ Index</t>
   </si>
   <si>
-    <t xml:space="preserve">102.211</t>
+    <t xml:space="preserve">121.441</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Ozone EJ Index</t>
@@ -3113,7 +3113,7 @@
     <t xml:space="preserve">US type of raw score for Wastewater Discharge EJ Index</t>
   </si>
   <si>
-    <t xml:space="preserve">10.821</t>
+    <t xml:space="preserve">10.825</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Drinking Water Non-Compliance EJ Index</t>
@@ -3125,7 +3125,7 @@
     <t xml:space="preserve">State type of raw score for Particulate Matter EJ Index</t>
   </si>
   <si>
-    <t xml:space="preserve">71.549</t>
+    <t xml:space="preserve">110.472</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Ozone EJ Index</t>
@@ -3161,7 +3161,7 @@
     <t xml:space="preserve">State type of raw score for Lead Paint EJ Index</t>
   </si>
   <si>
-    <t xml:space="preserve">143.981</t>
+    <t xml:space="preserve">143.983</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Superfund Proximity EJ Index</t>
@@ -3191,7 +3191,7 @@
     <t xml:space="preserve">State type of raw score for Wastewater Discharge EJ Index</t>
   </si>
   <si>
-    <t xml:space="preserve">12.69</t>
+    <t xml:space="preserve">12.691</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Drinking Water Non-Compliance EJ Index</t>
@@ -3203,7 +3203,7 @@
     <t xml:space="preserve">US type of raw score for Particulate Matter Supplemental EJ Index</t>
   </si>
   <si>
-    <t xml:space="preserve">103.974</t>
+    <t xml:space="preserve">122.523</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Ozone Supplemental EJ Index</t>
@@ -3269,7 +3269,7 @@
     <t xml:space="preserve">US type of raw score for Wastewater Discharge Supplemental EJ Index</t>
   </si>
   <si>
-    <t xml:space="preserve">14.408</t>
+    <t xml:space="preserve">14.414</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Drinking Water Non-Compliance Supplemental EJ Index</t>
@@ -3281,7 +3281,7 @@
     <t xml:space="preserve">State type of raw score for Particulate Matter Supplemental EJ Index</t>
   </si>
   <si>
-    <t xml:space="preserve">63.229</t>
+    <t xml:space="preserve">100.312</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Ozone Supplemental EJ Index</t>
@@ -3317,7 +3317,7 @@
     <t xml:space="preserve">State type of raw score for Lead Paint Supplemental EJ Index</t>
   </si>
   <si>
-    <t xml:space="preserve">128.182</t>
+    <t xml:space="preserve">128.183</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Superfund Proximity Supplemental EJ Index</t>
@@ -3347,7 +3347,7 @@
     <t xml:space="preserve">State type of raw score for Wastewater Discharge Supplemental EJ Index</t>
   </si>
   <si>
-    <t xml:space="preserve">14.285</t>
+    <t xml:space="preserve">14.286</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Drinking Water Non-Compliance Supplemental EJ Index</t>
@@ -5015,52 +5015,52 @@
         <v>868</v>
       </c>
       <c r="JJ1" s="17" t="s">
+        <v>869</v>
+      </c>
+      <c r="JK1" s="17" t="s">
         <v>870</v>
       </c>
-      <c r="JK1" s="17" t="s">
+      <c r="JL1" s="17" t="s">
         <v>871</v>
       </c>
-      <c r="JL1" s="17" t="s">
-        <v>872</v>
-      </c>
       <c r="JM1" s="17" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="JN1" s="17" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="JO1" s="17" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="JP1" s="17" t="s">
+        <v>879</v>
+      </c>
+      <c r="JQ1" s="17" t="s">
         <v>880</v>
       </c>
-      <c r="JQ1" s="17" t="s">
+      <c r="JR1" s="17" t="s">
         <v>881</v>
       </c>
-      <c r="JR1" s="17" t="s">
+      <c r="JS1" s="17" t="s">
         <v>882</v>
       </c>
-      <c r="JS1" s="17" t="s">
+      <c r="JT1" s="17" t="s">
         <v>883</v>
       </c>
-      <c r="JT1" s="17" t="s">
+      <c r="JU1" s="17" t="s">
         <v>884</v>
       </c>
-      <c r="JU1" s="17" t="s">
-        <v>885</v>
-      </c>
       <c r="JV1" s="17" t="s">
+        <v>886</v>
+      </c>
+      <c r="JW1" s="17" t="s">
         <v>887</v>
       </c>
-      <c r="JW1" s="17" t="s">
+      <c r="JX1" s="17" t="s">
         <v>888</v>
       </c>
-      <c r="JX1" s="17" t="s">
-        <v>889</v>
-      </c>
       <c r="JY1" s="17" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="JZ1" s="17" t="s">
         <v>892</v>
@@ -6243,7 +6243,7 @@
         <v>65</v>
       </c>
       <c r="JJ2" s="27" t="n">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="JK2" s="27" t="n">
         <v>45</v>
@@ -6282,7 +6282,7 @@
         <v>61</v>
       </c>
       <c r="JW2" s="27" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="JX2" s="27" t="n">
         <v>35</v>
@@ -6531,7 +6531,7 @@
         <v>76.952104370838</v>
       </c>
       <c r="NB2" s="23" t="n">
-        <v>7.10327117269274</v>
+        <v>22.4936920468603</v>
       </c>
       <c r="NC2" s="23" t="n">
         <v>40.0868661456388</v>
@@ -6555,7 +6555,7 @@
         <v>0</v>
       </c>
       <c r="NJ2" s="23" t="n">
-        <v>0.11220260640833</v>
+        <v>0.112202606408331</v>
       </c>
       <c r="NK2" s="23" t="n">
         <v>69.4594241523752</v>
@@ -6570,7 +6570,7 @@
         <v>32.5272085203054</v>
       </c>
       <c r="NO2" s="23" t="n">
-        <v>4.64674407432935</v>
+        <v>48.7908127804582</v>
       </c>
       <c r="NP2" s="23" t="n">
         <v>67.1034011881344</v>
@@ -6609,7 +6609,7 @@
         <v>88.2876496374691</v>
       </c>
       <c r="OB2" s="23" t="n">
-        <v>8.14962919730484</v>
+        <v>25.8071591247987</v>
       </c>
       <c r="OC2" s="23" t="n">
         <v>45.5515987340029</v>
@@ -6648,7 +6648,7 @@
         <v>29.6120790719457</v>
       </c>
       <c r="OO2" s="23" t="n">
-        <v>4.23029701027796</v>
+        <v>44.4181186079186</v>
       </c>
       <c r="OP2" s="23" t="n">
         <v>60.5340087444893</v>
@@ -7479,7 +7479,7 @@
         <v>78</v>
       </c>
       <c r="JJ3" s="27" t="n">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="JK3" s="27" t="n">
         <v>54</v>
@@ -7518,7 +7518,7 @@
         <v>83</v>
       </c>
       <c r="JW3" s="27" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="JX3" s="27" t="n">
         <v>48</v>
@@ -7767,7 +7767,7 @@
         <v>117.323328112055</v>
       </c>
       <c r="NB3" s="23" t="n">
-        <v>17.011654439911</v>
+        <v>3.14198123056293</v>
       </c>
       <c r="NC3" s="23" t="n">
         <v>55.4040107256464</v>
@@ -7806,7 +7806,7 @@
         <v>100.1875317907</v>
       </c>
       <c r="NO3" s="23" t="n">
-        <v>21.6245670015017</v>
+        <v>9.08260253494678</v>
       </c>
       <c r="NP3" s="23" t="n">
         <v>107.773014854969</v>
@@ -7845,7 +7845,7 @@
         <v>137.704563137612</v>
       </c>
       <c r="OB3" s="23" t="n">
-        <v>19.9724899609038</v>
+        <v>3.69086287583923</v>
       </c>
       <c r="OC3" s="23" t="n">
         <v>63.8425278565321</v>
@@ -7884,7 +7884,7 @@
         <v>116.075166654765</v>
       </c>
       <c r="OO3" s="23" t="n">
-        <v>24.9473534986623</v>
+        <v>10.5269105847758</v>
       </c>
       <c r="OP3" s="23" t="n">
         <v>123.809912115067</v>
@@ -8715,7 +8715,7 @@
         <v>49</v>
       </c>
       <c r="JJ4" s="27" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="JK4" s="27" t="n">
         <v>45</v>
@@ -8754,7 +8754,7 @@
         <v>55</v>
       </c>
       <c r="JW4" s="27" t="n">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="JX4" s="27" t="n">
         <v>51</v>
@@ -9003,7 +9003,7 @@
         <v>46.2569024602887</v>
       </c>
       <c r="NB4" s="23" t="n">
-        <v>53.1939097284581</v>
+        <v>57.7881992700524</v>
       </c>
       <c r="NC4" s="23" t="n">
         <v>40.6174315726002</v>
@@ -9015,7 +9015,7 @@
         <v>50.5458394252474</v>
       </c>
       <c r="NF4" s="23" t="n">
-        <v>25.6727508551648</v>
+        <v>25.6727508551649</v>
       </c>
       <c r="NG4" s="23" t="n">
         <v>32.4640947364053</v>
@@ -9042,7 +9042,7 @@
         <v>28.9204926360807</v>
       </c>
       <c r="NO4" s="23" t="n">
-        <v>32.4176693416491</v>
+        <v>30.1242536215768</v>
       </c>
       <c r="NP4" s="23" t="n">
         <v>25.5731126250819</v>
@@ -9081,13 +9081,13 @@
         <v>78.7006513591159</v>
       </c>
       <c r="OB4" s="23" t="n">
-        <v>90.4794216105559</v>
+        <v>98.2919233098529</v>
       </c>
       <c r="OC4" s="23" t="n">
         <v>68.6958772623984</v>
       </c>
       <c r="OD4" s="23" t="n">
-        <v>62.53628278916</v>
+        <v>62.5362827891599</v>
       </c>
       <c r="OE4" s="23" t="n">
         <v>85.95796252536</v>
@@ -9099,7 +9099,7 @@
         <v>54.3079386002305</v>
       </c>
       <c r="OH4" s="23" t="n">
-        <v>0.340712220215133</v>
+        <v>0.340712220215132</v>
       </c>
       <c r="OI4" s="23" t="n">
         <v>44.7075980646423</v>
@@ -9120,7 +9120,7 @@
         <v>40.0105653644774</v>
       </c>
       <c r="OO4" s="23" t="n">
-        <v>44.7470796119325</v>
+        <v>41.5311198776367</v>
       </c>
       <c r="OP4" s="23" t="n">
         <v>35.036702621778</v>
@@ -9951,7 +9951,7 @@
         <v>68</v>
       </c>
       <c r="JJ5" s="27" t="n">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="JK5" s="27" t="n">
         <v>64</v>
@@ -9990,7 +9990,7 @@
         <v>56</v>
       </c>
       <c r="JW5" s="27" t="n">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="JX5" s="27" t="n">
         <v>53</v>
@@ -10239,7 +10239,7 @@
         <v>85.7940962185773</v>
       </c>
       <c r="NB5" s="23" t="n">
-        <v>37.3024409358371</v>
+        <v>78.1608849503045</v>
       </c>
       <c r="NC5" s="23" t="n">
         <v>77.9065108076848</v>
@@ -10278,7 +10278,7 @@
         <v>58.3104575189475</v>
       </c>
       <c r="NO5" s="23" t="n">
-        <v>24.285683048698</v>
+        <v>39.3662659394878</v>
       </c>
       <c r="NP5" s="23" t="n">
         <v>83.7855642707251</v>
@@ -10314,10 +10314,10 @@
         <v>0</v>
       </c>
       <c r="OA5" s="23" t="n">
-        <v>79.2572403521155</v>
+        <v>79.2572403521154</v>
       </c>
       <c r="OB5" s="23" t="n">
-        <v>34.4713706018905</v>
+        <v>72.1947359100883</v>
       </c>
       <c r="OC5" s="23" t="n">
         <v>71.9788398868712</v>
@@ -10356,7 +10356,7 @@
         <v>41.0599362977923</v>
       </c>
       <c r="OO5" s="23" t="n">
-        <v>17.0860637170125</v>
+        <v>27.7031552536311</v>
       </c>
       <c r="OP5" s="23" t="n">
         <v>59.061514477926</v>
@@ -11187,7 +11187,7 @@
         <v>99</v>
       </c>
       <c r="JJ6" s="27" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="JK6" s="27" t="n">
         <v>98</v>
@@ -11475,7 +11475,7 @@
         <v>281.358733659431</v>
       </c>
       <c r="NB6" s="23" t="n">
-        <v>262.406396881789</v>
+        <v>282.909022125377</v>
       </c>
       <c r="NC6" s="23" t="n">
         <v>274.812565316584</v>
@@ -11514,7 +11514,7 @@
         <v>247.397482759081</v>
       </c>
       <c r="NO6" s="23" t="n">
-        <v>197.755366389805</v>
+        <v>240.32600179043</v>
       </c>
       <c r="NP6" s="23" t="n">
         <v>318.831826463656</v>
@@ -11553,7 +11553,7 @@
         <v>253.679355736826</v>
       </c>
       <c r="OB6" s="23" t="n">
-        <v>236.501124771856</v>
+        <v>254.985590802148</v>
       </c>
       <c r="OC6" s="23" t="n">
         <v>247.683878413021</v>
@@ -11592,7 +11592,7 @@
         <v>184.897571963874</v>
       </c>
       <c r="OO6" s="23" t="n">
-        <v>147.672115001314</v>
+        <v>179.344973662782</v>
       </c>
       <c r="OP6" s="23" t="n">
         <v>238.072938604179</v>
@@ -12423,7 +12423,7 @@
         <v>79</v>
       </c>
       <c r="JJ7" s="27" t="n">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="JK7" s="27" t="n">
         <v>94</v>
@@ -12462,7 +12462,7 @@
         <v>79</v>
       </c>
       <c r="JW7" s="27" t="n">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="JX7" s="27" t="n">
         <v>96</v>
@@ -12711,7 +12711,7 @@
         <v>119.342934038794</v>
       </c>
       <c r="NB7" s="23" t="n">
-        <v>120.693151951277</v>
+        <v>140.47556642207</v>
       </c>
       <c r="NC7" s="23" t="n">
         <v>226.881109944851</v>
@@ -12750,7 +12750,7 @@
         <v>214.490657324609</v>
       </c>
       <c r="NO7" s="23" t="n">
-        <v>82.2969344855926</v>
+        <v>166.375481097491</v>
       </c>
       <c r="NP7" s="23" t="n">
         <v>225.534652280655</v>
@@ -12789,7 +12789,7 @@
         <v>127.628782669497</v>
       </c>
       <c r="OB7" s="23" t="n">
-        <v>128.905833428549</v>
+        <v>150.258028876184</v>
       </c>
       <c r="OC7" s="23" t="n">
         <v>242.29122138924</v>
@@ -12828,7 +12828,7 @@
         <v>217.968064111516</v>
       </c>
       <c r="OO7" s="23" t="n">
-        <v>83.5408998486035</v>
+        <v>169.56437602125</v>
       </c>
       <c r="OP7" s="23" t="n">
         <v>228.543558431621</v>
@@ -13659,7 +13659,7 @@
         <v>92</v>
       </c>
       <c r="JJ8" s="27" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="JK8" s="27" t="n">
         <v>74</v>
@@ -13698,7 +13698,7 @@
         <v>90</v>
       </c>
       <c r="JW8" s="27" t="n">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="JX8" s="27" t="n">
         <v>67</v>
@@ -13947,7 +13947,7 @@
         <v>191.205018898703</v>
       </c>
       <c r="NB8" s="23" t="n">
-        <v>171.69430268455</v>
+        <v>165.841087820304</v>
       </c>
       <c r="NC8" s="23" t="n">
         <v>109.078326055277</v>
@@ -13986,7 +13986,7 @@
         <v>188.475055226975</v>
       </c>
       <c r="NO8" s="23" t="n">
-        <v>119.830003902458</v>
+        <v>81.9311902905521</v>
       </c>
       <c r="NP8" s="23" t="n">
         <v>81.229156086671</v>
@@ -14025,7 +14025,7 @@
         <v>167.951669108002</v>
       </c>
       <c r="OB8" s="23" t="n">
-        <v>150.813743688819</v>
+        <v>145.672366063063</v>
       </c>
       <c r="OC8" s="23" t="n">
         <v>99.0898348698581</v>
@@ -14064,7 +14064,7 @@
         <v>134.005453297153</v>
       </c>
       <c r="OO8" s="23" t="n">
-        <v>85.2020911262495</v>
+        <v>58.2491742039815</v>
       </c>
       <c r="OP8" s="23" t="n">
         <v>61.4445824420369</v>
@@ -14895,7 +14895,7 @@
         <v>27</v>
       </c>
       <c r="JJ9" s="27" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="JK9" s="27" t="n">
         <v>45</v>
@@ -14934,7 +14934,7 @@
         <v>30</v>
       </c>
       <c r="JW9" s="27" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="JX9" s="27" t="n">
         <v>57</v>
@@ -15183,7 +15183,7 @@
         <v>20.8338240073862</v>
       </c>
       <c r="NB9" s="23" t="n">
-        <v>16.2577007736515</v>
+        <v>13.6192087208813</v>
       </c>
       <c r="NC9" s="23" t="n">
         <v>41.5031106420557</v>
@@ -15216,13 +15216,13 @@
         <v>45.8075326573284</v>
       </c>
       <c r="NM9" s="23" t="n">
-        <v>54.3401515905647</v>
+        <v>54.4287172669241</v>
       </c>
       <c r="NN9" s="23" t="n">
         <v>76.8200246924354</v>
       </c>
       <c r="NO9" s="23" t="n">
-        <v>35.0423787864745</v>
+        <v>26.3966354599835</v>
       </c>
       <c r="NP9" s="23" t="n">
         <v>45.7650865975849</v>
@@ -15255,13 +15255,13 @@
         <v>83.4038301585497</v>
       </c>
       <c r="NZ9" s="23" t="n">
-        <v>76.027772567431</v>
+        <v>76.0498181113261</v>
       </c>
       <c r="OA9" s="23" t="n">
         <v>40.4442430955068</v>
       </c>
       <c r="OB9" s="23" t="n">
-        <v>31.4279734183963</v>
+        <v>26.2845715001041</v>
       </c>
       <c r="OC9" s="23" t="n">
         <v>78.3111587834872</v>
@@ -15294,13 +15294,13 @@
         <v>87.848543965725</v>
       </c>
       <c r="OM9" s="23" t="n">
-        <v>103.836739761746</v>
+        <v>103.948171527145</v>
       </c>
       <c r="ON9" s="23" t="n">
         <v>116.478675223817</v>
       </c>
       <c r="OO9" s="23" t="n">
-        <v>52.0940114253976</v>
+        <v>39.326312655874</v>
       </c>
       <c r="OP9" s="23" t="n">
         <v>67.140584360414</v>
@@ -15333,7 +15333,7 @@
         <v>125.494524497692</v>
       </c>
       <c r="OZ9" s="23" t="n">
-        <v>111.953235707364</v>
+        <v>111.986479534127</v>
       </c>
     </row>
     <row r="10">
@@ -16131,7 +16131,7 @@
         <v>40</v>
       </c>
       <c r="JJ10" s="27" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="JK10" s="27" t="n">
         <v>58</v>
@@ -16170,7 +16170,7 @@
         <v>32</v>
       </c>
       <c r="JW10" s="27" t="n">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="JX10" s="27" t="n">
         <v>57</v>
@@ -16419,7 +16419,7 @@
         <v>34.8367384887128</v>
       </c>
       <c r="NB10" s="23" t="n">
-        <v>95.4344294722853</v>
+        <v>91.7717841289426</v>
       </c>
       <c r="NC10" s="23" t="n">
         <v>63.5086082415396</v>
@@ -16431,7 +16431,7 @@
         <v>64.6306849495215</v>
       </c>
       <c r="NF10" s="23" t="n">
-        <v>56.9191126054963</v>
+        <v>56.9191126054964</v>
       </c>
       <c r="NG10" s="23" t="n">
         <v>65.9516507044135</v>
@@ -16452,13 +16452,13 @@
         <v>92.4504852183565</v>
       </c>
       <c r="NM10" s="23" t="n">
-        <v>32.127364837001</v>
+        <v>32.1273648370011</v>
       </c>
       <c r="NN10" s="23" t="n">
         <v>61.5902989919776</v>
       </c>
       <c r="NO10" s="23" t="n">
-        <v>46.2678173554966</v>
+        <v>100.32684917476</v>
       </c>
       <c r="NP10" s="23" t="n">
         <v>83.5823939937704</v>
@@ -16497,7 +16497,7 @@
         <v>43.3702089976161</v>
       </c>
       <c r="OB10" s="23" t="n">
-        <v>119.179945169641</v>
+        <v>114.544771853045</v>
       </c>
       <c r="OC10" s="23" t="n">
         <v>78.6296145938071</v>
@@ -16536,7 +16536,7 @@
         <v>52.5782117517509</v>
       </c>
       <c r="OO10" s="23" t="n">
-        <v>39.3051110813093</v>
+        <v>85.404451684061</v>
       </c>
       <c r="OP10" s="23" t="n">
         <v>71.0640541730264</v>
@@ -17367,7 +17367,7 @@
         <v>17</v>
       </c>
       <c r="JJ11" s="27" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="JK11" s="27" t="n">
         <v>23</v>
@@ -17406,7 +17406,7 @@
         <v>16</v>
       </c>
       <c r="JW11" s="27" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="JX11" s="27" t="n">
         <v>23</v>
@@ -17655,13 +17655,13 @@
         <v>11.4719784442551</v>
       </c>
       <c r="NB11" s="23" t="n">
-        <v>23.2810038753656</v>
+        <v>18.4020240303908</v>
       </c>
       <c r="NC11" s="23" t="n">
         <v>15.8294281365048</v>
       </c>
       <c r="ND11" s="23" t="n">
-        <v>27.2152039828163</v>
+        <v>27.2152039828164</v>
       </c>
       <c r="NE11" s="23" t="n">
         <v>22.7679456305678</v>
@@ -17670,7 +17670,7 @@
         <v>16.1729271888802</v>
       </c>
       <c r="NG11" s="23" t="n">
-        <v>30.8399700593177</v>
+        <v>30.8399700593178</v>
       </c>
       <c r="NH11" s="23" t="n">
         <v>12.8527927032356</v>
@@ -17682,10 +17682,10 @@
         <v>13.5146949461143</v>
       </c>
       <c r="NK11" s="23" t="n">
-        <v>33.3544873713657</v>
+        <v>33.3544873713658</v>
       </c>
       <c r="NL11" s="23" t="n">
-        <v>33.5890640983317</v>
+        <v>33.5890640983318</v>
       </c>
       <c r="NM11" s="23" t="n">
         <v>0</v>
@@ -17694,7 +17694,7 @@
         <v>11.2713427288303</v>
       </c>
       <c r="NO11" s="23" t="n">
-        <v>14.6021639810745</v>
+        <v>4.98471721830082</v>
       </c>
       <c r="NP11" s="23" t="n">
         <v>14.811463835389</v>
@@ -17712,7 +17712,7 @@
         <v>23.8865001827917</v>
       </c>
       <c r="NU11" s="23" t="n">
-        <v>2.12321394730008</v>
+        <v>2.17222936511013</v>
       </c>
       <c r="NV11" s="23" t="n">
         <v>0</v>
@@ -17733,7 +17733,7 @@
         <v>21.501400215027</v>
       </c>
       <c r="OB11" s="23" t="n">
-        <v>43.6582934703797</v>
+        <v>34.4809184087645</v>
       </c>
       <c r="OC11" s="23" t="n">
         <v>29.6242163063856</v>
@@ -17772,7 +17772,7 @@
         <v>16.8355873424264</v>
       </c>
       <c r="OO11" s="23" t="n">
-        <v>21.6983442716179</v>
+        <v>7.43027680185661</v>
       </c>
       <c r="OP11" s="23" t="n">
         <v>21.9720961019736</v>
@@ -17790,7 +17790,7 @@
         <v>35.6567565348414</v>
       </c>
       <c r="OU11" s="23" t="n">
-        <v>2.91339148915049</v>
+        <v>2.96472008395307</v>
       </c>
       <c r="OV11" s="23" t="n">
         <v>0</v>
@@ -18947,52 +18947,52 @@
         <v>868</v>
       </c>
       <c r="JH1" s="15" t="s">
+        <v>869</v>
+      </c>
+      <c r="JI1" s="17" t="s">
         <v>870</v>
       </c>
-      <c r="JI1" s="17" t="s">
+      <c r="JJ1" s="17" t="s">
         <v>871</v>
       </c>
-      <c r="JJ1" s="17" t="s">
-        <v>872</v>
-      </c>
       <c r="JK1" s="17" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="JL1" s="17" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="JM1" s="17" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="JN1" s="17" t="s">
+        <v>879</v>
+      </c>
+      <c r="JO1" s="17" t="s">
         <v>880</v>
       </c>
-      <c r="JO1" s="17" t="s">
+      <c r="JP1" s="17" t="s">
         <v>881</v>
       </c>
-      <c r="JP1" s="17" t="s">
+      <c r="JQ1" s="17" t="s">
         <v>882</v>
       </c>
-      <c r="JQ1" s="17" t="s">
+      <c r="JR1" s="17" t="s">
         <v>883</v>
       </c>
-      <c r="JR1" s="17" t="s">
+      <c r="JS1" s="17" t="s">
         <v>884</v>
       </c>
-      <c r="JS1" s="17" t="s">
-        <v>885</v>
-      </c>
       <c r="JT1" s="17" t="s">
+        <v>886</v>
+      </c>
+      <c r="JU1" s="17" t="s">
         <v>887</v>
       </c>
-      <c r="JU1" s="17" t="s">
+      <c r="JV1" s="17" t="s">
         <v>888</v>
       </c>
-      <c r="JV1" s="17" t="s">
-        <v>889</v>
-      </c>
       <c r="JW1" s="17" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="JX1" s="17" t="s">
         <v>892</v>
@@ -20173,7 +20173,7 @@
         <v>78</v>
       </c>
       <c r="JJ2" s="27" t="n">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="JK2" s="27" t="n">
         <v>83</v>
@@ -20212,7 +20212,7 @@
         <v>75</v>
       </c>
       <c r="JW2" s="27" t="n">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="JX2" s="27" t="n">
         <v>85</v>
@@ -20461,7 +20461,7 @@
         <v>117.312116899188</v>
       </c>
       <c r="NB2" s="23" t="n">
-        <v>102.211035118237</v>
+        <v>121.440843085412</v>
       </c>
       <c r="NC2" s="23" t="n">
         <v>147.749566513762</v>
@@ -20494,13 +20494,13 @@
         <v>109.501365093349</v>
       </c>
       <c r="NM2" s="23" t="n">
-        <v>10.8213053345218</v>
+        <v>10.8253658009493</v>
       </c>
       <c r="NN2" s="23" t="n">
         <v>142.891623579944</v>
       </c>
       <c r="NO2" s="23" t="n">
-        <v>71.5487559652744</v>
+        <v>110.471533216608</v>
       </c>
       <c r="NP2" s="23" t="n">
         <v>154.348158200293</v>
@@ -20518,7 +20518,7 @@
         <v>85.5078660379096</v>
       </c>
       <c r="NU2" s="23" t="n">
-        <v>143.981425622932</v>
+        <v>143.982618644189</v>
       </c>
       <c r="NV2" s="23" t="n">
         <v>162.213263447858</v>
@@ -20533,13 +20533,13 @@
         <v>108.36046751482</v>
       </c>
       <c r="NZ2" s="23" t="n">
-        <v>12.6896214220852</v>
+        <v>12.6906321431065</v>
       </c>
       <c r="OA2" s="23" t="n">
         <v>117.153378985886</v>
       </c>
       <c r="OB2" s="23" t="n">
-        <v>103.973930253546</v>
+        <v>122.523033390055</v>
       </c>
       <c r="OC2" s="23" t="n">
         <v>152.100205832046</v>
@@ -20554,7 +20554,7 @@
         <v>144.477633800058</v>
       </c>
       <c r="OG2" s="23" t="n">
-        <v>95.2776509351118</v>
+        <v>95.2776509351119</v>
       </c>
       <c r="OH2" s="23" t="n">
         <v>147.302056163125</v>
@@ -20572,13 +20572,13 @@
         <v>114.040127496428</v>
       </c>
       <c r="OM2" s="23" t="n">
-        <v>14.4084025793826</v>
+        <v>14.4135113863263</v>
       </c>
       <c r="ON2" s="23" t="n">
         <v>131.089527021018</v>
       </c>
       <c r="OO2" s="23" t="n">
-        <v>63.2289343780677</v>
+        <v>100.311668071496</v>
       </c>
       <c r="OP2" s="23" t="n">
         <v>139.762065830411</v>
@@ -20596,7 +20596,7 @@
         <v>74.1512036392973</v>
       </c>
       <c r="OU2" s="23" t="n">
-        <v>128.181612175162</v>
+        <v>128.182861498486</v>
       </c>
       <c r="OV2" s="23" t="n">
         <v>144.944179701337</v>
@@ -20611,7 +20611,7 @@
         <v>100.185422723694</v>
       </c>
       <c r="OZ2" s="23" t="n">
-        <v>14.2846356089992</v>
+        <v>14.2861597371721</v>
       </c>
     </row>
   </sheetData>
@@ -22905,10 +22905,10 @@
     </row>
     <row r="271">
       <c r="A271" t="s">
+        <v>668</v>
+      </c>
+      <c r="B271" t="s">
         <v>869</v>
-      </c>
-      <c r="B271" t="s">
-        <v>870</v>
       </c>
     </row>
     <row r="272">
@@ -22916,7 +22916,7 @@
         <v>671</v>
       </c>
       <c r="B272" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="273">
@@ -22924,39 +22924,39 @@
         <v>673</v>
       </c>
       <c r="B273" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="s">
+        <v>872</v>
+      </c>
+      <c r="B274" t="s">
         <v>873</v>
-      </c>
-      <c r="B274" t="s">
-        <v>874</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="s">
+        <v>874</v>
+      </c>
+      <c r="B275" t="s">
         <v>875</v>
-      </c>
-      <c r="B275" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="s">
+        <v>876</v>
+      </c>
+      <c r="B276" t="s">
         <v>877</v>
-      </c>
-      <c r="B276" t="s">
-        <v>878</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="s">
+        <v>878</v>
+      </c>
+      <c r="B277" t="s">
         <v>879</v>
-      </c>
-      <c r="B277" t="s">
-        <v>880</v>
       </c>
     </row>
     <row r="278">
@@ -22964,7 +22964,7 @@
         <v>671</v>
       </c>
       <c r="B278" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="279">
@@ -22972,15 +22972,15 @@
         <v>673</v>
       </c>
       <c r="B279" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B280" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="281">
@@ -22988,7 +22988,7 @@
         <v>642</v>
       </c>
       <c r="B281" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="282">
@@ -22996,23 +22996,23 @@
         <v>666</v>
       </c>
       <c r="B282" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="s">
+        <v>885</v>
+      </c>
+      <c r="B283" t="s">
         <v>886</v>
-      </c>
-      <c r="B283" t="s">
-        <v>887</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="s">
-        <v>877</v>
+        <v>786</v>
       </c>
       <c r="B284" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="285">
@@ -23020,20 +23020,20 @@
         <v>673</v>
       </c>
       <c r="B285" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="s">
+        <v>889</v>
+      </c>
+      <c r="B286" t="s">
         <v>890</v>
-      </c>
-      <c r="B286" t="s">
-        <v>891</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="s">
-        <v>869</v>
+        <v>891</v>
       </c>
       <c r="B287" t="s">
         <v>892</v>
@@ -23057,7 +23057,7 @@
     </row>
     <row r="290">
       <c r="A290" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B290" t="s">
         <v>896</v>
@@ -23065,7 +23065,7 @@
     </row>
     <row r="291">
       <c r="A291" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B291" t="s">
         <v>897</v>
@@ -23073,7 +23073,7 @@
     </row>
     <row r="292">
       <c r="A292" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B292" t="s">
         <v>898</v>

</xml_diff>

<commit_message>
Tests Pass: recreated testoutput_ejamit... and fixed a test
</commit_message>
<xml_diff>
--- a/inst/testdata/examples_of_output/testoutput_ejamit_10pts_1miles.xlsx
+++ b/inst/testdata/examples_of_output/testoutput_ejamit_10pts_1miles.xlsx
@@ -2207,72 +2207,75 @@
     <t xml:space="preserve">State percentile for % Asian (non-Hispanic, single race)</t>
   </si>
   <si>
+    <t xml:space="preserve">State percentile for % American Indian and Alaska Native (non-Hispanic, single race)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State percentile for % Native Hawaiian and Other Pacific Islander (non-Hispanic, single race)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State percentile for % Other race (non-Hispanic, single race)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State percentile for % Two or more races (non-Hispanic)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State percentile for % White (non-Hispanic, single race)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State percentile for % with Disabilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State percentile for %Low life expectancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Average for Demographic Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Average for Supplemental EJ Index for Supplemental Demographic Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Average for % Low Income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Average for % in limited English-speaking Households</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Average for % Unemployed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Average for % with Less Than High School Education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Average for % under Age 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Average for % over Age 64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Average for % People of Color</t>
+  </si>
+  <si>
     <t xml:space="preserve">26</t>
   </si>
   <si>
-    <t xml:space="preserve">State percentile for % American Indian and Alaska Native (non-Hispanic, single race)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State percentile for % Native Hawaiian and Other Pacific Islander (non-Hispanic, single race)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State percentile for % Other race (non-Hispanic, single race)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State percentile for % Two or more races (non-Hispanic)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State percentile for % White (non-Hispanic, single race)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State percentile for % with Disabilities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State percentile for %Low life expectancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Average for Demographic Index</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Average for Supplemental EJ Index for Supplemental Demographic Index</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Average for % Low Income</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Average for % in limited English-speaking Households</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Average for % Unemployed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Average for % with Less Than High School Education</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Average for % under Age 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Average for % over Age 64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Average for % People of Color</t>
-  </si>
-  <si>
     <t xml:space="preserve">State Average for % Hispanic or Latino</t>
   </si>
   <si>
@@ -2531,13 +2534,16 @@
     <t xml:space="preserve">State percentile for Superfund Proximity (site count/km distance)</t>
   </si>
   <si>
+    <t xml:space="preserve">82</t>
+  </si>
+  <si>
     <t xml:space="preserve">State percentile for RMP Proximity (facility count/km distance)</t>
   </si>
   <si>
     <t xml:space="preserve">State percentile for Hazardous Waste Proximity (facility count/km distance)</t>
   </si>
   <si>
-    <t xml:space="preserve">44</t>
+    <t xml:space="preserve">47</t>
   </si>
   <si>
     <t xml:space="preserve">State percentile for Underground Storage Tanks (UST) indicator</t>
@@ -2645,9 +2651,6 @@
     <t xml:space="preserve">US percentile for EJ Index for Toxic Releases to Air</t>
   </si>
   <si>
-    <t xml:space="preserve">82</t>
-  </si>
-  <si>
     <t xml:space="preserve">US percentile for EJ Index for Traffic Proximity and Volume</t>
   </si>
   <si>
@@ -2655,9 +2658,6 @@
   </si>
   <si>
     <t xml:space="preserve">US percentile for EJ Index for Lead Paint Indicator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">86</t>
   </si>
   <si>
     <t xml:space="preserve">US percentile for EJ Index for Superfund Proximity</t>
@@ -4739,10 +4739,10 @@
         <v>727</v>
       </c>
       <c r="FV1" s="12" t="s">
+        <v>728</v>
+      </c>
+      <c r="FW1" s="12" t="s">
         <v>729</v>
-      </c>
-      <c r="FW1" s="12" t="s">
-        <v>730</v>
       </c>
       <c r="FX1" s="12" t="s">
         <v>731</v>
@@ -4787,250 +4787,250 @@
         <v>749</v>
       </c>
       <c r="GL1" s="8" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="GM1" s="8" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="GN1" s="8" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="GO1" s="8" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="GP1" s="8" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="GQ1" s="8" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="GR1" s="8" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="GS1" s="8" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="GT1" s="8" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="GU1" s="8" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="GV1" s="13" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="GW1" s="13" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="GX1" s="13" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="GY1" s="13" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="GZ1" s="13" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="HA1" s="13" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="HB1" s="13" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="HC1" s="13" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="HD1" s="13" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="HE1" s="13" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="HF1" s="13" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="HG1" s="13" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="HH1" s="13" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="HI1" s="14" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="HJ1" s="14" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="HK1" s="14" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="HL1" s="14" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="HM1" s="14" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="HN1" s="14" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="HO1" s="14" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="HP1" s="14" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="HQ1" s="14" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="HR1" s="14" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="HS1" s="14" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="HT1" s="14" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="HU1" s="14" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="HV1" s="15" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="HW1" s="15" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="HX1" s="15" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="HY1" s="15" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="HZ1" s="15" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="IA1" s="15" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="IB1" s="15" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="IC1" s="15" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="ID1" s="15" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="IE1" s="15" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="IF1" s="15" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="IG1" s="15" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="IH1" s="15" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="II1" s="16" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="IJ1" s="16" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="IK1" s="16" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="IL1" s="16" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="IM1" s="16" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="IN1" s="16" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="IO1" s="16" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="IP1" s="16" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="IQ1" s="16" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="IR1" s="16" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="IS1" s="16" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="IT1" s="16" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="IU1" s="16" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="IV1" s="15" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="IW1" s="15" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="IX1" s="15" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="IY1" s="15" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="IZ1" s="15" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
       <c r="JA1" s="15" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="JB1" s="15" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="JC1" s="15" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="JD1" s="15" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="JE1" s="15" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="JF1" s="15" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="JG1" s="15" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="JH1" s="15" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="JI1" s="17" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="JJ1" s="17" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="JK1" s="17" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="JL1" s="17" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="JM1" s="17" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="JN1" s="17" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="JO1" s="17" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="JP1" s="17" t="s">
         <v>879</v>
@@ -6191,10 +6191,10 @@
         <v>0</v>
       </c>
       <c r="IR2" s="27" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="IS2" s="27" t="n">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="IT2" s="27" t="n">
         <v>10</v>
@@ -7209,13 +7209,13 @@
         <v>82</v>
       </c>
       <c r="FV3" s="27" t="n">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="FW3" s="27" t="n">
         <v>0</v>
       </c>
       <c r="FX3" s="27" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="FY3" s="27" t="n">
         <v>61</v>
@@ -7424,13 +7424,13 @@
         <v>0</v>
       </c>
       <c r="IQ3" s="27" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="IR3" s="27" t="n">
         <v>0</v>
       </c>
       <c r="IS3" s="27" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="IT3" s="27" t="n">
         <v>65</v>
@@ -8657,7 +8657,7 @@
         <v>32</v>
       </c>
       <c r="IP4" s="27" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="IQ4" s="27" t="n">
         <v>15</v>
@@ -8666,7 +8666,7 @@
         <v>55</v>
       </c>
       <c r="IS4" s="27" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="IT4" s="27" t="n">
         <v>21</v>
@@ -9681,13 +9681,13 @@
         <v>74</v>
       </c>
       <c r="FV5" s="27" t="n">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="FW5" s="27" t="n">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="FX5" s="27" t="n">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="FY5" s="27" t="n">
         <v>82</v>
@@ -9893,10 +9893,10 @@
         <v>54</v>
       </c>
       <c r="IP5" s="27" t="n">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="IQ5" s="27" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="IR5" s="27" t="n">
         <v>89</v>
@@ -10920,7 +10920,7 @@
         <v>84</v>
       </c>
       <c r="FW6" s="27" t="n">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="FX6" s="27" t="n">
         <v>83</v>
@@ -11129,7 +11129,7 @@
         <v>87</v>
       </c>
       <c r="IP6" s="27" t="n">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="IQ6" s="27" t="n">
         <v>99</v>
@@ -12153,13 +12153,13 @@
         <v>52</v>
       </c>
       <c r="FV7" s="27" t="n">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="FW7" s="27" t="n">
         <v>0</v>
       </c>
       <c r="FX7" s="27" t="n">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="FY7" s="27" t="n">
         <v>82</v>
@@ -12365,10 +12365,10 @@
         <v>31</v>
       </c>
       <c r="IP7" s="27" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="IQ7" s="27" t="n">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="IR7" s="27" t="n">
         <v>93</v>
@@ -13601,7 +13601,7 @@
         <v>25</v>
       </c>
       <c r="IP8" s="27" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="IQ8" s="27" t="n">
         <v>93</v>
@@ -17309,7 +17309,7 @@
         <v>49</v>
       </c>
       <c r="IP11" s="27" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="IQ11" s="27" t="n">
         <v>0</v>
@@ -18671,10 +18671,10 @@
         <v>727</v>
       </c>
       <c r="FT1" s="12" t="s">
+        <v>728</v>
+      </c>
+      <c r="FU1" s="12" t="s">
         <v>729</v>
-      </c>
-      <c r="FU1" s="12" t="s">
-        <v>730</v>
       </c>
       <c r="FV1" s="12" t="s">
         <v>731</v>
@@ -18719,250 +18719,250 @@
         <v>749</v>
       </c>
       <c r="GJ1" s="8" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="GK1" s="8" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="GL1" s="8" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="GM1" s="8" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="GN1" s="8" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="GO1" s="8" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="GP1" s="8" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="GQ1" s="8" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="GR1" s="8" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="GS1" s="8" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="GT1" s="8" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="GU1" s="8" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="GV1" s="13" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="GW1" s="13" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="GX1" s="13" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="GY1" s="13" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="GZ1" s="13" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="HA1" s="13" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="HB1" s="13" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="HC1" s="13" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="HD1" s="13" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="HE1" s="13" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="HF1" s="13" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="HG1" s="13" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="HH1" s="13" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="HI1" s="14" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="HJ1" s="14" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="HK1" s="14" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="HL1" s="14" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="HM1" s="14" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="HN1" s="14" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="HO1" s="14" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="HP1" s="14" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="HQ1" s="14" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="HR1" s="14" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="HS1" s="14" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="HT1" s="14" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="HU1" s="14" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="HV1" s="15" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="HW1" s="15" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="HX1" s="15" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="HY1" s="15" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="HZ1" s="15" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="IA1" s="15" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="IB1" s="15" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="IC1" s="15" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="ID1" s="15" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="IE1" s="15" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="IF1" s="15" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="IG1" s="15" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="IH1" s="15" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="II1" s="16" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="IJ1" s="16" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="IK1" s="16" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="IL1" s="16" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="IM1" s="16" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="IN1" s="16" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="IO1" s="16" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="IP1" s="16" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="IQ1" s="16" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="IR1" s="16" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="IS1" s="16" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="IT1" s="16" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="IU1" s="16" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="IV1" s="15" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="IW1" s="15" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="IX1" s="15" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
       <c r="IY1" s="15" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="IZ1" s="15" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="JA1" s="15" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="JB1" s="15" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="JC1" s="15" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="JD1" s="15" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="JE1" s="15" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="JF1" s="15" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="JG1" s="15" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="JH1" s="15" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="JI1" s="17" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="JJ1" s="17" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="JK1" s="17" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="JL1" s="17" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="JM1" s="17" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="JN1" s="17" t="s">
         <v>879</v>
@@ -19903,13 +19903,13 @@
         <v>57.6216050626212</v>
       </c>
       <c r="FV2" s="27" t="n">
-        <v>26.0844119852241</v>
+        <v>84.9423601169581</v>
       </c>
       <c r="FW2" s="27" t="n">
-        <v>5.02618445096331</v>
+        <v>37.931634588221</v>
       </c>
       <c r="FX2" s="27" t="n">
-        <v>26.3473274981435</v>
+        <v>85.612347469941</v>
       </c>
       <c r="FY2" s="27" t="n">
         <v>68.8657580521925</v>
@@ -20115,16 +20115,16 @@
         <v>46.4249874543021</v>
       </c>
       <c r="IP2" s="27" t="n">
-        <v>3.76963833822248</v>
+        <v>69.7121730817598</v>
       </c>
       <c r="IQ2" s="27" t="n">
-        <v>26.6169908681623</v>
+        <v>82.3314591272486</v>
       </c>
       <c r="IR2" s="27" t="n">
-        <v>78.9323777941743</v>
+        <v>79.1870584420925</v>
       </c>
       <c r="IS2" s="27" t="n">
-        <v>43.5815947161454</v>
+        <v>47.1976415279885</v>
       </c>
       <c r="IT2" s="27" t="n">
         <v>60.1564576670604</v>
@@ -22175,23 +22175,23 @@
     </row>
     <row r="179">
       <c r="A179" t="s">
+        <v>673</v>
+      </c>
+      <c r="B179" t="s">
         <v>728</v>
-      </c>
-      <c r="B179" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>593</v>
+        <v>682</v>
       </c>
       <c r="B180" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="B181" t="s">
         <v>731</v>
@@ -22303,10 +22303,10 @@
     </row>
     <row r="195">
       <c r="A195" t="s">
-        <v>728</v>
+        <v>750</v>
       </c>
       <c r="B195" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
     </row>
     <row r="196">
@@ -22314,7 +22314,7 @@
         <v>588</v>
       </c>
       <c r="B196" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="197">
@@ -22322,7 +22322,7 @@
         <v>3</v>
       </c>
       <c r="B197" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="198">
@@ -22330,7 +22330,7 @@
         <v>522</v>
       </c>
       <c r="B198" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
     </row>
     <row r="199">
@@ -22338,7 +22338,7 @@
         <v>522</v>
       </c>
       <c r="B199" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
     </row>
     <row r="200">
@@ -22346,7 +22346,7 @@
         <v>7</v>
       </c>
       <c r="B200" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
     </row>
     <row r="201">
@@ -22354,7 +22354,7 @@
         <v>704</v>
       </c>
       <c r="B201" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
     </row>
     <row r="202">
@@ -22362,15 +22362,15 @@
         <v>646</v>
       </c>
       <c r="B202" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="B203" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="204">
@@ -22378,71 +22378,71 @@
         <v>638</v>
       </c>
       <c r="B204" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B205" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B206" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B207" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="B208" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B209" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B210" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="B211" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="B212" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="213">
@@ -22450,37 +22450,37 @@
         <v>531</v>
       </c>
       <c r="B213" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B214" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="B215" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="B216" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
     </row>
     <row r="217">
       <c r="A217"/>
       <c r="B217" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
     </row>
     <row r="218">
@@ -22488,31 +22488,31 @@
         <v>659</v>
       </c>
       <c r="B218" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B219" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="B220" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="B221" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
     </row>
     <row r="222">
@@ -22520,7 +22520,7 @@
         <v>654</v>
       </c>
       <c r="B222" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
     </row>
     <row r="223">
@@ -22528,15 +22528,15 @@
         <v>659</v>
       </c>
       <c r="B223" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="B224" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
     </row>
     <row r="225">
@@ -22544,7 +22544,7 @@
         <v>677</v>
       </c>
       <c r="B225" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
     </row>
     <row r="226">
@@ -22552,7 +22552,7 @@
         <v>677</v>
       </c>
       <c r="B226" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
     </row>
     <row r="227">
@@ -22560,15 +22560,15 @@
         <v>675</v>
       </c>
       <c r="B227" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B228" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
     </row>
     <row r="229">
@@ -22576,61 +22576,61 @@
         <v>649</v>
       </c>
       <c r="B229" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
     </row>
     <row r="230">
       <c r="A230"/>
       <c r="B230" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B231" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="B232" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="B233" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="B234" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="B235" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B236" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
     </row>
     <row r="237">
@@ -22638,23 +22638,23 @@
         <v>543</v>
       </c>
       <c r="B237" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="B238" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="B239" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
     </row>
     <row r="240">
@@ -22662,23 +22662,23 @@
         <v>516</v>
       </c>
       <c r="B240" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="B241" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="B242" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
     </row>
     <row r="243">
@@ -22686,7 +22686,7 @@
         <v>507</v>
       </c>
       <c r="B243" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
     </row>
     <row r="244">
@@ -22694,15 +22694,15 @@
         <v>654</v>
       </c>
       <c r="B244" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B245" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
     </row>
     <row r="246">
@@ -22710,15 +22710,15 @@
         <v>642</v>
       </c>
       <c r="B246" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B247" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
     </row>
     <row r="248">
@@ -22726,7 +22726,7 @@
         <v>642</v>
       </c>
       <c r="B248" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
     </row>
     <row r="249">
@@ -22734,47 +22734,47 @@
         <v>654</v>
       </c>
       <c r="B249" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="B250" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="s">
-        <v>514</v>
+        <v>654</v>
       </c>
       <c r="B251" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="s">
-        <v>604</v>
+        <v>837</v>
       </c>
       <c r="B252" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B253" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="B254" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
     </row>
     <row r="255">
@@ -22782,117 +22782,117 @@
         <v>706</v>
       </c>
       <c r="B255" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
     </row>
     <row r="256">
       <c r="A256"/>
       <c r="B256" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="B257" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="B258" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="B259" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="B260" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="B261" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="B262" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="B263" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="B264" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="B265" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="B266" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="B267" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="B268" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="B269" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
     </row>
     <row r="270">
@@ -22900,7 +22900,7 @@
         <v>649</v>
       </c>
       <c r="B270" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
     </row>
     <row r="271">
@@ -22908,7 +22908,7 @@
         <v>668</v>
       </c>
       <c r="B271" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
     </row>
     <row r="272">
@@ -22916,7 +22916,7 @@
         <v>671</v>
       </c>
       <c r="B272" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
     </row>
     <row r="273">
@@ -22924,36 +22924,36 @@
         <v>673</v>
       </c>
       <c r="B273" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="B274" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="s">
-        <v>874</v>
+        <v>837</v>
       </c>
       <c r="B275" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="B276" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="s">
-        <v>878</v>
+        <v>730</v>
       </c>
       <c r="B277" t="s">
         <v>879</v>
@@ -22977,7 +22977,7 @@
     </row>
     <row r="280">
       <c r="A280" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="B280" t="s">
         <v>882</v>
@@ -23009,7 +23009,7 @@
     </row>
     <row r="284">
       <c r="A284" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B284" t="s">
         <v>887</v>
@@ -23057,7 +23057,7 @@
     </row>
     <row r="290">
       <c r="A290" t="s">
-        <v>878</v>
+        <v>730</v>
       </c>
       <c r="B290" t="s">
         <v>896</v>
@@ -23065,7 +23065,7 @@
     </row>
     <row r="291">
       <c r="A291" t="s">
-        <v>874</v>
+        <v>837</v>
       </c>
       <c r="B291" t="s">
         <v>897</v>
@@ -23073,7 +23073,7 @@
     </row>
     <row r="292">
       <c r="A292" t="s">
-        <v>878</v>
+        <v>730</v>
       </c>
       <c r="B292" t="s">
         <v>898</v>
@@ -23401,7 +23401,7 @@
     </row>
     <row r="333">
       <c r="A333" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B333" t="s">
         <v>954</v>

</xml_diff>